<commit_message>
RPM based prediction implemented
</commit_message>
<xml_diff>
--- a/pred_hv_comp.xlsx
+++ b/pred_hv_comp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul\Downloads\VickersHardnessPrediction-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul\Downloads\Vicker-s-Micro-Hardness-ANN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A8EA8C-3F84-4C3A-A7F2-93D8FEBBD26C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B59D48-EBF6-485B-A2BD-0B3ABB0234D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{68D17003-87CC-4B25-BE76-3113C3B74C40}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Composition</t>
   </si>
   <si>
     <t>Ag0.05Gd0.048Pd0.902 </t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>CaCO3</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BCD37CB-522A-44F7-8760-4C0AF9F709FE}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,6 +406,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
new RPM module added
</commit_message>
<xml_diff>
--- a/pred_hv_comp.xlsx
+++ b/pred_hv_comp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\VickersHardnessPrediction-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul\Desktop\Vicker-s-Micro-Hardness-ANN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACDA4052-3B5F-4F3C-83DC-5F184EEF608C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352F4E5B-4213-4E9C-8FF8-5778D4E9F523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15975" yWindow="4215" windowWidth="12825" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8850" yWindow="1470" windowWidth="12825" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Composition</t>
   </si>
   <si>
     <t>B3C10N3</t>
-  </si>
-  <si>
-    <t>LaSi2</t>
-  </si>
-  <si>
-    <t>WSi2</t>
-  </si>
-  <si>
-    <t>ScB2C2</t>
   </si>
 </sst>
 </file>
@@ -357,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,21 +371,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>